<commit_message>
fix numerical issue with simulation by changing input step function to logistic function. calculate angular velocity and acceleration and verify motor is capable of driving system. add datasheets for possible stepper motor.
</commit_message>
<xml_diff>
--- a/system_parameters.xlsx
+++ b/system_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Desktop\ball_on_beam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738CC177-6E67-4EEE-B6DA-7E4FDFD7966C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087375B1-B05E-4436-8085-3EE9B62B741C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8574" yWindow="7314" windowWidth="17280" windowHeight="10524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="14478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>parameters</t>
   </si>
   <si>
@@ -45,21 +42,32 @@
     <t>note</t>
   </si>
   <si>
-    <t>angular velocity 10^15 during step response</t>
-  </si>
-  <si>
-    <t>based on advice from James Viollete, 10^14 angular velocity during step respons</t>
-  </si>
-  <si>
-    <t>PID Tuner for 2 response time and 0.6 robustness</t>
+    <t>angular velocity 8000 during response to 0.10</t>
+  </si>
+  <si>
+    <t>PID Tuner for 2 response time and 0.6 robustness, but the issue is its tuning for a step t o 1, and I'm only stepping to 0.1</t>
+  </si>
+  <si>
+    <t>based on advice from James Viollete, 1000 angular velocity during step respons</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,9 +95,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,25 +388,25 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -414,7 +423,7 @@
         <v>-8</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -422,16 +431,16 @@
         <v>45660</v>
       </c>
       <c r="B6">
-        <v>-0.01</v>
+        <v>-3.2627999999999997E-2</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>-1.8881E-3</v>
       </c>
       <c r="D6">
-        <v>-1</v>
+        <v>-0.14096</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -439,19 +448,20 @@
         <v>45660</v>
       </c>
       <c r="B7">
-        <v>-3.2627999999999997E-2</v>
+        <v>-0.01</v>
       </c>
       <c r="C7">
-        <v>-1.8881E-3</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>-0.14096</v>
+        <v>-1</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add motor, track, base, support to 3d model
</commit_message>
<xml_diff>
--- a/system_parameters.xlsx
+++ b/system_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Desktop\ball_on_beam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087375B1-B05E-4436-8085-3EE9B62B741C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D07807-B794-4E92-A144-D24E6F31D993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="14478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>parameters</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">step </t>
+  </si>
+  <si>
+    <t>pid tuner -- peak: -0.6 theta, 20 omega, 0.3 torque</t>
   </si>
 </sst>
 </file>
@@ -379,23 +385,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:E7"/>
+  <dimension ref="A3:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -408,8 +414,11 @@
       <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>45660</v>
       </c>
@@ -422,11 +431,11 @@
       <c r="D5">
         <v>-8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>45660</v>
       </c>
@@ -439,11 +448,11 @@
       <c r="D6">
         <v>-0.14096</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>45660</v>
       </c>
@@ -456,8 +465,28 @@
       <c r="D7">
         <v>-1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1">
+        <v>45661</v>
+      </c>
+      <c r="B8">
+        <v>-0.14788000000000001</v>
+      </c>
+      <c r="D8">
+        <v>-0.30982999999999999</v>
+      </c>
+      <c r="E8">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>